<commit_message>
4090 small triangle은 일단 포기.
</commit_message>
<xml_diff>
--- a/_draft0/tomoGPU.xlsx
+++ b/_draft0/tomoGPU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\__TomoNV_Projects\Tomo_GPU2024\_draft0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11ABBB8-18BA-4922-BDE5-78FFC4A4E292}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BAF235-5114-4500-9CA7-0461A8BB4BB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="19860" activeTab="2" xr2:uid="{B3C603CF-1766-43DF-9F47-8A0B621A15C8}"/>
   </bookViews>
@@ -11772,7 +11772,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
2024-07-10 일단 본문 작성.
</commit_message>
<xml_diff>
--- a/_draft0/tomoGPU.xlsx
+++ b/_draft0/tomoGPU.xlsx
@@ -8,18 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\__TomoNV_Projects\Tomo_GPU2024\_draft0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61639147-E767-48C5-AA16-8ECDE5FC25CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CE4330-8136-4E55-8871-477B84A8F775}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="형상별Mtotal" sheetId="5" r:id="rId1"/>
-    <sheet name="임계각별Mtotal" sheetId="3" r:id="rId2"/>
-    <sheet name="HW별속도" sheetId="4" r:id="rId3"/>
+    <sheet name="B_2x" sheetId="6" r:id="rId2"/>
+    <sheet name="임계각별Mtotal" sheetId="3" r:id="rId3"/>
+    <sheet name="HW별속도" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -346,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="159">
   <si>
     <t>50x50x50</t>
   </si>
@@ -1106,16 +1104,21 @@
   <si>
     <t>GPU</t>
   </si>
+  <si>
+    <t>slicer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="177" formatCode="0.0_);[Red]\(0.0\)"/>
+    <numFmt numFmtId="178" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1298,6 +1301,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1470,15 +1481,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1668,14 +1682,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1686,11 +1703,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="백분율" xfId="2" builtinId="5"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
@@ -9260,796 +9278,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="형상별Mtotal"/>
-      <sheetName val="임계각별Mtotal"/>
-      <sheetName val="HW별속도"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="Y1" t="str">
-            <v>Mo</v>
-          </cell>
-          <cell r="Z1" t="str">
-            <v>Mss</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="W2" t="str">
-            <v>#1
-cube</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="X3" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y3">
-            <v>35.6</v>
-          </cell>
-          <cell r="Z3">
-            <v>3.2</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="X4" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y4">
-            <v>35.03</v>
-          </cell>
-          <cell r="Z4">
-            <v>2.4900000000000002</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="X5" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y5">
-            <v>35.03</v>
-          </cell>
-          <cell r="Z5">
-            <v>1.37</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="W7" t="str">
-            <v>#2
-sphere</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="X8" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y8">
-            <v>58.8</v>
-          </cell>
-          <cell r="Z8">
-            <v>2.4</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="X9" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y9">
-            <v>54.59</v>
-          </cell>
-          <cell r="Z9">
-            <v>2.23</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="X10" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y10">
-            <v>52.83</v>
-          </cell>
-          <cell r="Z10">
-            <v>1.53</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="W12" t="str">
-            <v>#3
-cone</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="X13" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y13">
-            <v>73.599999999999994</v>
-          </cell>
-          <cell r="Z13">
-            <v>9.1</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="X14" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y14">
-            <v>67.66</v>
-          </cell>
-          <cell r="Z14">
-            <v>7.45</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="X15" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y15">
-            <v>67.069999999999993</v>
-          </cell>
-          <cell r="Z15">
-            <v>3.14</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="W17" t="str">
-            <v>#4
-Bx2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="X18" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y18">
-            <v>181.4</v>
-          </cell>
-          <cell r="Z18">
-            <v>26.6</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="X19" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y19">
-            <v>170.31</v>
-          </cell>
-          <cell r="Z19">
-            <v>20.92</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="X20" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y20">
-            <v>170.67</v>
-          </cell>
-          <cell r="Z20">
-            <v>17.190000000000001</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="W22" t="str">
-            <v>#5
-B</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="X23" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y23">
-            <v>29</v>
-          </cell>
-          <cell r="Z23">
-            <v>5.0999999999999996</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="X24" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y24">
-            <v>27.07</v>
-          </cell>
-          <cell r="Z24">
-            <v>3.89</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="X25" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y25">
-            <v>26.86</v>
-          </cell>
-          <cell r="Z25">
-            <v>3.11</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="W27" t="str">
-            <v>#6
-Bx0.5</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="X28" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y28">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="Z28">
-            <v>1.2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="X29" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y29">
-            <v>4.84</v>
-          </cell>
-          <cell r="Z29">
-            <v>0.87</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="X30" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y30">
-            <v>4.6900000000000004</v>
-          </cell>
-          <cell r="Z30">
-            <v>0.75</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="W32" t="str">
-            <v>#7
-B/5k</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="X33" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y33">
-            <v>28.9</v>
-          </cell>
-          <cell r="Z33">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="X34" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y34">
-            <v>26.82</v>
-          </cell>
-          <cell r="Z34">
-            <v>4.12</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="X35" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y35">
-            <v>26.6</v>
-          </cell>
-          <cell r="Z35">
-            <v>3.13</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="W37" t="str">
-            <v>#8
-B/1k</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="X38" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y38">
-            <v>28.8</v>
-          </cell>
-          <cell r="Z38">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="X39" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y39">
-            <v>26.7</v>
-          </cell>
-          <cell r="Z39">
-            <v>3.83</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="X40" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y40">
-            <v>26.51</v>
-          </cell>
-          <cell r="Z40">
-            <v>1.71</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="W42" t="str">
-            <v>#9
-mnk</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="X43" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y43">
-            <v>22.3</v>
-          </cell>
-          <cell r="Z43">
-            <v>11.3</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="X44" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y44">
-            <v>22.8</v>
-          </cell>
-          <cell r="Z44">
-            <v>5.87</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="X45" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y45">
-            <v>22.9</v>
-          </cell>
-          <cell r="Z45">
-            <v>4.91</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="W47" t="str">
-            <v>#10
-drg</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="X48" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y48">
-            <v>96</v>
-          </cell>
-          <cell r="Z48">
-            <v>24.4</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="K49" t="str">
-            <v>Mss</v>
-          </cell>
-          <cell r="N49" t="str">
-            <v>Mo</v>
-          </cell>
-          <cell r="X49" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y49">
-            <v>87.97</v>
-          </cell>
-          <cell r="Z49">
-            <v>17.940000000000001</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="K50" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="L50" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="M50" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="N50" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="O50" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="P50" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="X50" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y50">
-            <v>87.22</v>
-          </cell>
-          <cell r="Z50">
-            <v>14.62</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="J51" t="str">
-            <v>#1
-cube</v>
-          </cell>
-          <cell r="K51">
-            <v>38.800000000000004</v>
-          </cell>
-          <cell r="L51">
-            <v>37.520000000000003</v>
-          </cell>
-          <cell r="M51">
-            <v>36.4</v>
-          </cell>
-          <cell r="N51">
-            <v>35.6</v>
-          </cell>
-          <cell r="O51">
-            <v>35.03</v>
-          </cell>
-          <cell r="P51">
-            <v>35.03</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="J52" t="str">
-            <v>#2
-sphere</v>
-          </cell>
-          <cell r="K52">
-            <v>61.199999999999996</v>
-          </cell>
-          <cell r="L52">
-            <v>56.82</v>
-          </cell>
-          <cell r="M52">
-            <v>54.36</v>
-          </cell>
-          <cell r="N52">
-            <v>58.8</v>
-          </cell>
-          <cell r="O52">
-            <v>54.59</v>
-          </cell>
-          <cell r="P52">
-            <v>52.83</v>
-          </cell>
-          <cell r="W52" t="str">
-            <v>#11
-Buda</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="J53" t="str">
-            <v>#3
-cone</v>
-          </cell>
-          <cell r="K53">
-            <v>82.699999999999989</v>
-          </cell>
-          <cell r="L53">
-            <v>75.11</v>
-          </cell>
-          <cell r="M53">
-            <v>70.209999999999994</v>
-          </cell>
-          <cell r="N53">
-            <v>73.599999999999994</v>
-          </cell>
-          <cell r="O53">
-            <v>67.66</v>
-          </cell>
-          <cell r="P53">
-            <v>67.069999999999993</v>
-          </cell>
-          <cell r="X53" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y53">
-            <v>38.299999999999997</v>
-          </cell>
-          <cell r="Z53">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="J54" t="str">
-            <v>#4
-Bx2</v>
-          </cell>
-          <cell r="K54">
-            <v>208</v>
-          </cell>
-          <cell r="L54">
-            <v>191.23000000000002</v>
-          </cell>
-          <cell r="M54">
-            <v>187.85999999999999</v>
-          </cell>
-          <cell r="N54">
-            <v>181.4</v>
-          </cell>
-          <cell r="O54">
-            <v>170.31</v>
-          </cell>
-          <cell r="P54">
-            <v>170.67</v>
-          </cell>
-          <cell r="X54" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y54">
-            <v>37.130000000000003</v>
-          </cell>
-          <cell r="Z54">
-            <v>10.7</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="J55" t="str">
-            <v>#5
-B</v>
-          </cell>
-          <cell r="K55">
-            <v>34.1</v>
-          </cell>
-          <cell r="L55">
-            <v>30.96</v>
-          </cell>
-          <cell r="M55">
-            <v>29.97</v>
-          </cell>
-          <cell r="N55">
-            <v>29</v>
-          </cell>
-          <cell r="O55">
-            <v>27.07</v>
-          </cell>
-          <cell r="P55">
-            <v>26.86</v>
-          </cell>
-          <cell r="X55" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y55">
-            <v>35.6</v>
-          </cell>
-          <cell r="Z55">
-            <v>5.72</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="J56" t="str">
-            <v>#6
-Bx0.5</v>
-          </cell>
-          <cell r="K56">
-            <v>6.3</v>
-          </cell>
-          <cell r="L56">
-            <v>5.71</v>
-          </cell>
-          <cell r="M56">
-            <v>5.44</v>
-          </cell>
-          <cell r="N56">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="O56">
-            <v>4.84</v>
-          </cell>
-          <cell r="P56">
-            <v>4.6900000000000004</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="J57" t="str">
-            <v>#7
-B/5k</v>
-          </cell>
-          <cell r="K57">
-            <v>33.9</v>
-          </cell>
-          <cell r="L57">
-            <v>30.94</v>
-          </cell>
-          <cell r="M57">
-            <v>29.73</v>
-          </cell>
-          <cell r="N57">
-            <v>28.9</v>
-          </cell>
-          <cell r="O57">
-            <v>26.82</v>
-          </cell>
-          <cell r="P57">
-            <v>26.6</v>
-          </cell>
-          <cell r="W57" t="str">
-            <v>#12
-Lucy</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="J58" t="str">
-            <v>#8
-B/1k</v>
-          </cell>
-          <cell r="K58">
-            <v>33.799999999999997</v>
-          </cell>
-          <cell r="L58">
-            <v>30.53</v>
-          </cell>
-          <cell r="M58">
-            <v>28.220000000000002</v>
-          </cell>
-          <cell r="N58">
-            <v>28.8</v>
-          </cell>
-          <cell r="O58">
-            <v>26.7</v>
-          </cell>
-          <cell r="P58">
-            <v>26.51</v>
-          </cell>
-          <cell r="X58" t="str">
-            <v>Slicer</v>
-          </cell>
-          <cell r="Y58">
-            <v>50.9</v>
-          </cell>
-          <cell r="Z58">
-            <v>10.8</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="J59" t="str">
-            <v>#9
-mnk</v>
-          </cell>
-          <cell r="K59">
-            <v>33.6</v>
-          </cell>
-          <cell r="L59">
-            <v>28.67</v>
-          </cell>
-          <cell r="M59">
-            <v>27.81</v>
-          </cell>
-          <cell r="N59">
-            <v>22.3</v>
-          </cell>
-          <cell r="O59">
-            <v>22.8</v>
-          </cell>
-          <cell r="P59">
-            <v>22.9</v>
-          </cell>
-          <cell r="X59" t="str">
-            <v>CPU</v>
-          </cell>
-          <cell r="Y59">
-            <v>48.86</v>
-          </cell>
-          <cell r="Z59">
-            <v>4.79</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="J60" t="str">
-            <v>#10
-drg</v>
-          </cell>
-          <cell r="K60">
-            <v>120.4</v>
-          </cell>
-          <cell r="L60">
-            <v>105.91</v>
-          </cell>
-          <cell r="M60">
-            <v>101.84</v>
-          </cell>
-          <cell r="N60">
-            <v>96</v>
-          </cell>
-          <cell r="O60">
-            <v>87.97</v>
-          </cell>
-          <cell r="P60">
-            <v>87.22</v>
-          </cell>
-          <cell r="X60" t="str">
-            <v>GPU</v>
-          </cell>
-          <cell r="Y60">
-            <v>49.06</v>
-          </cell>
-          <cell r="Z60">
-            <v>5.19</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="J61" t="str">
-            <v>#11
-Buda</v>
-          </cell>
-          <cell r="K61">
-            <v>46.3</v>
-          </cell>
-          <cell r="L61">
-            <v>47.83</v>
-          </cell>
-          <cell r="M61">
-            <v>41.32</v>
-          </cell>
-          <cell r="N61">
-            <v>38.299999999999997</v>
-          </cell>
-          <cell r="O61">
-            <v>37.130000000000003</v>
-          </cell>
-          <cell r="P61">
-            <v>35.6</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="J62" t="str">
-            <v>#12
-Lucy</v>
-          </cell>
-          <cell r="K62">
-            <v>61.7</v>
-          </cell>
-          <cell r="L62">
-            <v>53.65</v>
-          </cell>
-          <cell r="M62">
-            <v>54.25</v>
-          </cell>
-          <cell r="N62">
-            <v>50.9</v>
-          </cell>
-          <cell r="O62">
-            <v>48.86</v>
-          </cell>
-          <cell r="P62">
-            <v>49.06</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -10349,8 +9577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436D07ED-6439-43D2-9403-4BF5002283BA}">
   <dimension ref="B1:AE77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView topLeftCell="C9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -10410,7 +9638,7 @@
       <c r="N2" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="63"/>
+      <c r="O2" s="66"/>
       <c r="P2" s="62" t="s">
         <v>57</v>
       </c>
@@ -10656,7 +9884,7 @@
         <v>91</v>
       </c>
       <c r="D7" s="60"/>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="63" t="s">
         <v>116</v>
       </c>
       <c r="F7" s="60" t="s">
@@ -10708,7 +9936,7 @@
         <v>92</v>
       </c>
       <c r="D8" s="60"/>
-      <c r="E8" s="64"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="60" t="s">
         <v>3</v>
       </c>
@@ -10763,7 +9991,7 @@
         <v>93</v>
       </c>
       <c r="D9" s="60"/>
-      <c r="E9" s="64"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="60" t="s">
         <v>4</v>
       </c>
@@ -11635,16 +10863,16 @@
       </c>
     </row>
     <row r="49" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="C49" s="69" t="s">
+      <c r="C49" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="69"/>
-      <c r="E49" s="69"/>
-      <c r="F49" s="69" t="s">
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="G49" s="69"/>
-      <c r="H49" s="69"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
       <c r="K49" t="s">
         <v>153</v>
       </c>
@@ -12735,6 +11963,78 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2529F582-12F9-4FAE-BD1D-DB64E7EC6B45}">
+  <dimension ref="B3:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>181.4</v>
+      </c>
+      <c r="D4">
+        <v>169.8</v>
+      </c>
+      <c r="E4" s="70">
+        <f>(D4-$C4)/$C4</f>
+        <v>-6.3947078280044062E-2</v>
+      </c>
+      <c r="F4">
+        <v>170.4</v>
+      </c>
+      <c r="G4" s="70">
+        <f>(F4-$C4)/$C4</f>
+        <v>-6.0639470782800436E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>26.4</v>
+      </c>
+      <c r="D5">
+        <v>20.7</v>
+      </c>
+      <c r="E5" s="70">
+        <f>(D5-$C5)/$C5</f>
+        <v>-0.21590909090909088</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
+      <c r="G5" s="70">
+        <f>(F5-$C5)/$C5</f>
+        <v>-0.35606060606060602</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:M17"/>
   <sheetViews>
@@ -12757,26 +12057,26 @@
     <row r="2" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="21"/>
       <c r="B2" s="28"/>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66" t="s">
+      <c r="F2" s="67"/>
+      <c r="G2" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="J2" s="66" t="s">
+      <c r="H2" s="67"/>
+      <c r="J2" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66" t="s">
+      <c r="K2" s="67"/>
+      <c r="L2" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="66"/>
+      <c r="M2" s="67"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="22" t="s">
@@ -13219,7 +12519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
@@ -13524,7 +12824,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="26.4" x14ac:dyDescent="0.4">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="68" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -13535,7 +12835,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="68"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -13588,13 +12888,13 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="68" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="68" t="s">
         <v>15</v>
       </c>
       <c r="D18" t="s">
@@ -13602,11 +12902,11 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="68"/>
+      <c r="A19" s="69"/>
       <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="68"/>
+      <c r="C19" s="69"/>
       <c r="D19" s="18" t="s">
         <v>123</v>
       </c>

</xml_diff>